<commit_message>
boton de guardar para los reportes anexo 7  boleta de valorizacion petroperu Lote I IV  Z69 y general.
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletadeValorizacionPetroperuLoteZ69.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/mensual/BoletadeValorizacionPetroperuLoteZ69.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\SP\APSS SP\ProyectoPrincipalAenza5\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\mensual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC8273B3-6D0F-4A5C-AFBA-E2EC4BFF5FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5747628-B8E9-451B-8DF6-5F0AFD00A6CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -774,6 +774,9 @@
     <xf numFmtId="166" fontId="9" fillId="0" borderId="1" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -845,9 +848,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="104">
@@ -1350,7 +1350,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1368,52 +1368,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="26" t="s">
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="U1" s="27"/>
+      <c r="U1" s="28"/>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="28" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="30"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="U2" s="28"/>
+      <c r="U2" s="29"/>
     </row>
     <row r="3" spans="2:21" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="19" t="s">
@@ -1426,30 +1426,30 @@
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
-      <c r="I3" s="47" t="s">
+      <c r="I3" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="34"/>
-      <c r="L3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="36"/>
     </row>
     <row r="4" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="30" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="31"/>
-      <c r="L4" s="32"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="33"/>
     </row>
     <row r="5" spans="2:21" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="4"/>
@@ -1471,7 +1471,7 @@
       <c r="H5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I5" s="48"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="14" t="s">
         <v>8</v>
       </c>
@@ -1510,7 +1510,7 @@
       </c>
     </row>
     <row r="6" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="22" t="s">
@@ -1634,11 +1634,11 @@
       <c r="I10" s="6"/>
     </row>
     <row r="11" spans="2:21" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="45"/>
-      <c r="D11" s="46"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="47"/>
       <c r="E11" s="24" t="s">
         <v>42</v>
       </c>
@@ -1649,8 +1649,8 @@
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="44"/>
     </row>
     <row r="13" spans="2:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1"/>
@@ -1659,21 +1659,21 @@
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="2:21" ht="37.799999999999997" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="18" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="15" spans="2:21" ht="42.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="42"/>
       <c r="E15" s="18" t="s">
         <v>46</v>
       </c>
@@ -1694,25 +1694,25 @@
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>